<commit_message>
update main program for caommunication to PLC Slave
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLMAN\MF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27025D7C-516C-4F63-82FA-403E00C7B002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE563DBD-0523-416C-80FB-F5C7CBAD11F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="182">
   <si>
     <t>Effective Length</t>
   </si>
@@ -459,15 +459,6 @@
     <t>M23</t>
   </si>
   <si>
-    <t>Jog Feeding Request</t>
-  </si>
-  <si>
-    <t>Jog Bending Request</t>
-  </si>
-  <si>
-    <t>Jog Turning Request</t>
-  </si>
-  <si>
     <t>M30</t>
   </si>
   <si>
@@ -553,6 +544,33 @@
   </si>
   <si>
     <t>Request</t>
+  </si>
+  <si>
+    <t>Jog Feeding Request Positif</t>
+  </si>
+  <si>
+    <t>M27</t>
+  </si>
+  <si>
+    <t>M28</t>
+  </si>
+  <si>
+    <t>Jog Feeding Request Negatif</t>
+  </si>
+  <si>
+    <t>M29</t>
+  </si>
+  <si>
+    <t>Jog Bending Request Positif</t>
+  </si>
+  <si>
+    <t>Jog Bending Request Negatif</t>
+  </si>
+  <si>
+    <t>Jog Turning Request Positif</t>
+  </si>
+  <si>
+    <t>Jog Turning Request Negatif</t>
   </si>
 </sst>
 </file>
@@ -887,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,7 +986,7 @@
         <v>50</v>
       </c>
       <c r="L8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M8">
         <v>3072</v>
@@ -977,10 +995,10 @@
         <v>123</v>
       </c>
       <c r="O8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="P8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
@@ -1012,7 +1030,7 @@
         <v>127</v>
       </c>
       <c r="O9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P9" t="s">
         <v>137</v>
@@ -1038,7 +1056,7 @@
         <v>128</v>
       </c>
       <c r="O10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P10" t="s">
         <v>126</v>
@@ -1064,19 +1082,19 @@
         <v>52</v>
       </c>
       <c r="L11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M11">
         <v>3075</v>
       </c>
       <c r="N11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
@@ -1119,7 +1137,7 @@
         <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M13">
         <v>3082</v>
@@ -1128,10 +1146,10 @@
         <v>129</v>
       </c>
       <c r="O13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="P13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
@@ -1154,7 +1172,7 @@
         <v>55</v>
       </c>
       <c r="L14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M14">
         <v>3083</v>
@@ -1163,10 +1181,10 @@
         <v>130</v>
       </c>
       <c r="O14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="P14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -1198,21 +1216,21 @@
         <v>131</v>
       </c>
       <c r="O15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C16">
         <v>2520</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G16" t="s">
         <v>85</v>
@@ -1233,10 +1251,10 @@
         <v>132</v>
       </c>
       <c r="O16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
@@ -1279,10 +1297,10 @@
         <v>140</v>
       </c>
       <c r="O18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
@@ -1305,7 +1323,7 @@
         <v>60</v>
       </c>
       <c r="L19" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="M19">
         <v>3093</v>
@@ -1314,10 +1332,10 @@
         <v>141</v>
       </c>
       <c r="O19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
@@ -1340,7 +1358,7 @@
         <v>70</v>
       </c>
       <c r="L20" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="M20">
         <v>3094</v>
@@ -1349,10 +1367,10 @@
         <v>142</v>
       </c>
       <c r="O20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
@@ -1366,7 +1384,7 @@
         <v>36</v>
       </c>
       <c r="L21" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="M21">
         <v>3095</v>
@@ -1375,10 +1393,10 @@
         <v>143</v>
       </c>
       <c r="O21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
@@ -1392,19 +1410,19 @@
         <v>37</v>
       </c>
       <c r="L22" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="M22">
         <v>3096</v>
       </c>
       <c r="N22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
@@ -1427,19 +1445,19 @@
         <v>78</v>
       </c>
       <c r="L23" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="M23">
         <v>3097</v>
       </c>
       <c r="N23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
@@ -1462,19 +1480,19 @@
         <v>80</v>
       </c>
       <c r="L24" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="M24">
         <v>3098</v>
       </c>
       <c r="N24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
@@ -1487,6 +1505,21 @@
       <c r="D25" t="s">
         <v>40</v>
       </c>
+      <c r="L25" t="s">
+        <v>166</v>
+      </c>
+      <c r="M25">
+        <v>3099</v>
+      </c>
+      <c r="N25" t="s">
+        <v>174</v>
+      </c>
+      <c r="O25" t="s">
+        <v>160</v>
+      </c>
+      <c r="P25" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -1508,19 +1541,19 @@
         <v>86</v>
       </c>
       <c r="L26" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="M26">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="N26" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="O26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
@@ -1542,6 +1575,21 @@
       <c r="I27" t="s">
         <v>87</v>
       </c>
+      <c r="L27" t="s">
+        <v>168</v>
+      </c>
+      <c r="M27">
+        <v>3101</v>
+      </c>
+      <c r="N27" t="s">
+        <v>177</v>
+      </c>
+      <c r="O27" t="s">
+        <v>160</v>
+      </c>
+      <c r="P27" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -1581,6 +1629,21 @@
       </c>
       <c r="I29" t="s">
         <v>89</v>
+      </c>
+      <c r="L29" t="s">
+        <v>134</v>
+      </c>
+      <c r="M29">
+        <v>3102</v>
+      </c>
+      <c r="N29" t="s">
+        <v>144</v>
+      </c>
+      <c r="O29" t="s">
+        <v>160</v>
+      </c>
+      <c r="P29" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update plc programs and variables
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4987274E-D63C-4953-B35A-88A68C1E1297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C90DC3-71B9-4D48-842F-B5DA5D3BB69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VAR" sheetId="1" r:id="rId1"/>
+    <sheet name="IO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
   <si>
     <t>Effective Length</t>
   </si>
@@ -583,6 +584,171 @@
   </si>
   <si>
     <t>Coils</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>Button SV ON</t>
+  </si>
+  <si>
+    <t>Button Run</t>
+  </si>
+  <si>
+    <t>Button Stop</t>
+  </si>
+  <si>
+    <t>Button Emergency</t>
+  </si>
+  <si>
+    <t>High Speed Counter A Servo Turn</t>
+  </si>
+  <si>
+    <t>High Speed Counter B Servo Turn</t>
+  </si>
+  <si>
+    <t>High Speed Counter A Servo Feed</t>
+  </si>
+  <si>
+    <t>High Speed Counter B Servo Feed</t>
+  </si>
+  <si>
+    <t>High Speed Counter A Servo Bend</t>
+  </si>
+  <si>
+    <t>High Speed Counter B Servo Bend</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Y0</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Servo On Turn</t>
+  </si>
+  <si>
+    <t>Servo On Feed</t>
+  </si>
+  <si>
+    <t>Servo On Bend</t>
+  </si>
+  <si>
+    <t>Relay Servo Contactor</t>
+  </si>
+  <si>
+    <t>Relay Hydraulic Pump Contactor</t>
+  </si>
+  <si>
+    <t>Lamp 01</t>
+  </si>
+  <si>
+    <t>Lamp 02</t>
+  </si>
+  <si>
+    <t>Lamp 03</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Chuck</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Clamp</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Mandrel</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Pressure Positive</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Pressure Negative</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Y8</t>
+  </si>
+  <si>
+    <t>Y9</t>
+  </si>
+  <si>
+    <t>Y10</t>
+  </si>
+  <si>
+    <t>Y11</t>
+  </si>
+  <si>
+    <t>Y12</t>
+  </si>
+  <si>
+    <t>Chuck</t>
+  </si>
+  <si>
+    <t>Mandrel</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>At Front</t>
+  </si>
+  <si>
+    <t>At Back</t>
   </si>
 </sst>
 </file>
@@ -649,11 +815,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:Q30"/>
+    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,1086 +1119,1122 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="L6" s="1" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="1" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2512</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>3512</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>3072</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>2513</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>3513</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>3073</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="Q9" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>2514</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="L10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="2">
         <v>3074</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q10" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>2515</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>3523</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="2">
         <v>3075</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="Q11" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2516</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>3524</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>2517</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>3525</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="2">
         <v>3082</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>2518</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>3526</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="2">
         <v>3083</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>2519</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>3527</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3084</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2520</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3528</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="M16" s="2">
+        <v>3085</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3529</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M15" s="3">
-        <v>3084</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="M17" s="2">
+        <v>3086</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P17" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="Q17" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2520</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3528</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="3" t="s">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2522</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3530</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M16" s="3">
-        <v>3085</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="M18" s="2">
+        <v>3087</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P18" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q18" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="3">
-        <v>3529</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2522</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="3">
-        <v>3530</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="3" t="s">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2523</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3531</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2524</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3532</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M20" s="2">
         <v>3092</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="N20" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O20" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="P20" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="Q20" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2523</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="3">
-        <v>3531</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" s="3" t="s">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2525</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="L21" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M21" s="2">
         <v>3093</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N21" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O21" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="P21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="Q21" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2524</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="3">
-        <v>3532</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="3" t="s">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2526</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="L22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M22" s="2">
         <v>3094</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="N22" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="O22" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="P22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="Q22" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2525</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="L21" s="3" t="s">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2527</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3542</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M23" s="2">
         <v>3095</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="N23" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="O23" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="P23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q23" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="3">
-        <v>2526</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="L22" s="3" t="s">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2528</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3543</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M24" s="2">
         <v>3096</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="N24" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="O24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="P24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q22" s="3" t="s">
+      <c r="Q24" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2527</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="3">
-        <v>3542</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="3" t="s">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2529</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="L25" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M25" s="2">
         <v>3097</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="N25" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O25" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="P25" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q23" s="3" t="s">
+      <c r="Q25" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2528</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="3">
-        <v>3543</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L24" s="3" t="s">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2530</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3553</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M26" s="2">
         <v>3098</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="N26" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O26" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="P26" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q24" s="3" t="s">
+      <c r="Q26" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2529</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="L25" s="3" t="s">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2531</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="2">
+        <v>3554</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M27" s="2">
         <v>3099</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="P27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q25" s="3" t="s">
+      <c r="Q27" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2530</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="3">
-        <v>3553</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L26" s="3" t="s">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2532</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="2">
+        <v>3555</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M28" s="2">
         <v>3100</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N28" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="P28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="Q28" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2531</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3554</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L27" s="3" t="s">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2533</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3556</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M29" s="2">
         <v>3101</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="N29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="O29" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="P29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q27" s="3" t="s">
+      <c r="Q29" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="3">
-        <v>2532</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="3">
-        <v>3555</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="3">
-        <v>2533</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="3">
-        <v>3556</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L29" s="3" t="s">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2534</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3557</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2535</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3558</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M31" s="2">
         <v>3102</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="N31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="P31" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="Q31" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3">
-        <v>2534</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H30" s="3">
-        <v>3557</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2535</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H31" s="3">
-        <v>3558</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>2536</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>3559</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="G33" s="3" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>3560</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>3561</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
         <v>3562</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>3572</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>3573</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>3583</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>3584</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I42" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>3585</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>3586</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>3587</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <v>3588</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <v>3589</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>3590</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="I48" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>3591</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="I49" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>3592</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="I50" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2044,4 +2246,524 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B135286-D673-4043-B681-3A5B7A012B1D}">
+  <dimension ref="B6:N30"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="6" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="13" width="10.21875" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="I6:N6"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update plc and main program for configuration
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C90DC3-71B9-4D48-842F-B5DA5D3BB69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128A9ABB-D8EA-4C83-BFA1-32FD90D345FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="364">
   <si>
     <t>Effective Length</t>
   </si>
@@ -749,6 +749,375 @@
   </si>
   <si>
     <t>At Back</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Present Value</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value</t>
+  </si>
+  <si>
+    <t>V3111</t>
+  </si>
+  <si>
+    <t>V3112</t>
+  </si>
+  <si>
+    <t>V3113</t>
+  </si>
+  <si>
+    <t>V3114</t>
+  </si>
+  <si>
+    <t>V3115</t>
+  </si>
+  <si>
+    <t>V3116</t>
+  </si>
+  <si>
+    <t>V3117</t>
+  </si>
+  <si>
+    <t>V3118</t>
+  </si>
+  <si>
+    <t>V3119</t>
+  </si>
+  <si>
+    <t>V3120</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 1</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 2</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 3</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 4</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 5</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 6</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 7</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 8</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 9</t>
+  </si>
+  <si>
+    <t>Feeding Speed Config Set Value Step 10</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Present Value</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 1</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 2</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 3</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 4</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 5</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 6</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 7</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 8</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 9</t>
+  </si>
+  <si>
+    <t>Bending Speed Config Set Value Step 10</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Present Value</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 1</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 2</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 3</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 4</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 5</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 6</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 7</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 8</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 9</t>
+  </si>
+  <si>
+    <t>Turning Speed Config Set Value Step 10</t>
+  </si>
+  <si>
+    <t>Y13</t>
+  </si>
+  <si>
+    <t>Y14</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Table Up</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Hydraulic Table Down</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 1</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 2</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 3</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 4</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 5</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 6</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 7</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 8</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 9</t>
+  </si>
+  <si>
+    <t>Feeding Linear Offset from Bending Step 10</t>
+  </si>
+  <si>
+    <t>V3200</t>
+  </si>
+  <si>
+    <t>V3201</t>
+  </si>
+  <si>
+    <t>V3211</t>
+  </si>
+  <si>
+    <t>V3212</t>
+  </si>
+  <si>
+    <t>V3213</t>
+  </si>
+  <si>
+    <t>V3214</t>
+  </si>
+  <si>
+    <t>V3215</t>
+  </si>
+  <si>
+    <t>V3216</t>
+  </si>
+  <si>
+    <t>V3217</t>
+  </si>
+  <si>
+    <t>V3218</t>
+  </si>
+  <si>
+    <t>V3219</t>
+  </si>
+  <si>
+    <t>V3220</t>
+  </si>
+  <si>
+    <t>V3230</t>
+  </si>
+  <si>
+    <t>V3231</t>
+  </si>
+  <si>
+    <t>V3241</t>
+  </si>
+  <si>
+    <t>V3242</t>
+  </si>
+  <si>
+    <t>V3243</t>
+  </si>
+  <si>
+    <t>V3244</t>
+  </si>
+  <si>
+    <t>V3245</t>
+  </si>
+  <si>
+    <t>V3246</t>
+  </si>
+  <si>
+    <t>V3247</t>
+  </si>
+  <si>
+    <t>V3248</t>
+  </si>
+  <si>
+    <t>V3249</t>
+  </si>
+  <si>
+    <t>V3250</t>
+  </si>
+  <si>
+    <t>V3260</t>
+  </si>
+  <si>
+    <t>V3261</t>
+  </si>
+  <si>
+    <t>V3271</t>
+  </si>
+  <si>
+    <t>V3272</t>
+  </si>
+  <si>
+    <t>V3273</t>
+  </si>
+  <si>
+    <t>V3274</t>
+  </si>
+  <si>
+    <t>V3275</t>
+  </si>
+  <si>
+    <t>V3276</t>
+  </si>
+  <si>
+    <t>V3277</t>
+  </si>
+  <si>
+    <t>V3278</t>
+  </si>
+  <si>
+    <t>V3279</t>
+  </si>
+  <si>
+    <t>V3280</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 1</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 2</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 3</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 4</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 5</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 6</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 7</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 8</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 9</t>
+  </si>
+  <si>
+    <t>Bed Position Config Step 10</t>
+  </si>
+  <si>
+    <t>Bed Position Config Present Value</t>
+  </si>
+  <si>
+    <t>Bed Position Config Set Value</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Actuator</t>
+  </si>
+  <si>
+    <t>M300</t>
+  </si>
+  <si>
+    <t>M301</t>
+  </si>
+  <si>
+    <t>M311</t>
+  </si>
+  <si>
+    <t>M312</t>
+  </si>
+  <si>
+    <t>M313</t>
+  </si>
+  <si>
+    <t>M314</t>
+  </si>
+  <si>
+    <t>M315</t>
+  </si>
+  <si>
+    <t>M316</t>
+  </si>
+  <si>
+    <t>M317</t>
+  </si>
+  <si>
+    <t>M318</t>
+  </si>
+  <si>
+    <t>M319</t>
+  </si>
+  <si>
+    <t>M320</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:Q51"/>
+  <dimension ref="B6:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41:X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,13 +1481,17 @@
     <col min="3" max="4" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15.33203125" customWidth="1"/>
-    <col min="12" max="12" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.88671875" customWidth="1"/>
     <col min="13" max="14" width="15.33203125" customWidth="1"/>
-    <col min="15" max="16" width="10.21875" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="17" max="17" width="33.6640625" customWidth="1"/>
+    <col min="18" max="19" width="15.33203125" customWidth="1"/>
+    <col min="22" max="22" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.33203125" customWidth="1"/>
+    <col min="25" max="26" width="10.21875" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>124</v>
       </c>
@@ -1130,15 +1503,25 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="V6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1158,7 +1541,7 @@
         <v>24</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>23</v>
@@ -1166,17 +1549,35 @@
       <c r="N7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1195,26 +1596,38 @@
       <c r="I8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="R8" s="2">
+        <v>3712</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="2">
+      <c r="W8" s="2">
         <v>3072</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1233,26 +1646,38 @@
       <c r="I9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="R9" s="2">
+        <v>3713</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="V9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M9" s="2">
+      <c r="W9" s="2">
         <v>3073</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="Y9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="AA9" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1265,26 +1690,32 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="V10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="2">
+      <c r="W10" s="2">
         <v>3074</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Z10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="AA10" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1304,25 +1735,43 @@
         <v>52</v>
       </c>
       <c r="L11" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3623</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="R11" s="2">
+        <v>3723</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="V11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M11" s="2">
+      <c r="W11" s="2">
         <v>3075</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="Y11" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Z11" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="AA11" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1341,14 +1790,32 @@
       <c r="I12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L12" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="M12" s="2">
+        <v>3624</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="R12" s="2">
+        <v>3724</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1368,25 +1835,43 @@
         <v>54</v>
       </c>
       <c r="L13" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="M13" s="2">
+        <v>3625</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="R13" s="2">
+        <v>3725</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="V13" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M13" s="2">
+      <c r="W13" s="2">
         <v>3082</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="Y13" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1406,25 +1891,43 @@
         <v>55</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3626</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="R14" s="2">
+        <v>3726</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="V14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="M14" s="2">
+      <c r="W14" s="2">
         <v>3083</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="Y14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="AA14" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1444,25 +1947,43 @@
         <v>56</v>
       </c>
       <c r="L15" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3627</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="R15" s="2">
+        <v>3727</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="M15" s="2">
+      <c r="W15" s="2">
         <v>3084</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="Y15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Z15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="AA15" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>163</v>
       </c>
@@ -1482,25 +2003,43 @@
         <v>57</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M16" s="2">
+        <v>3628</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="R16" s="2">
+        <v>3728</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="M16" s="2">
+      <c r="W16" s="2">
         <v>3085</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="Y16" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Z16" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="AA16" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1514,25 +2053,43 @@
         <v>58</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="M17" s="2">
+        <v>3629</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="R17" s="2">
+        <v>3729</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="V17" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="2">
+      <c r="W17" s="2">
         <v>3086</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="Y17" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="AA17" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1552,25 +2109,43 @@
         <v>59</v>
       </c>
       <c r="L18" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="M18" s="2">
+        <v>3630</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="R18" s="2">
+        <v>3730</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="V18" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M18" s="2">
+      <c r="W18" s="2">
         <v>3087</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="Y18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1589,14 +2164,32 @@
       <c r="I19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L19" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3631</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="R19" s="2">
+        <v>3731</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1616,25 +2209,43 @@
         <v>70</v>
       </c>
       <c r="L20" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M20" s="2">
+        <v>3632</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R20" s="2">
+        <v>3732</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="V20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M20" s="2">
+      <c r="W20" s="2">
         <v>3092</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="X20" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="Y20" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="Z20" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="AA20" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
@@ -1647,26 +2258,32 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="L21" s="2" t="s">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="V21" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M21" s="2">
+      <c r="W21" s="2">
         <v>3093</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="Y21" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1679,26 +2296,32 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="V22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M22" s="2">
+      <c r="W22" s="2">
         <v>3094</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="X22" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="Y22" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="Z22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="AA22" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1717,26 +2340,38 @@
       <c r="I23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="Q23" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="R23" s="2">
+        <v>3742</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="V23" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M23" s="2">
+      <c r="W23" s="2">
         <v>3095</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="Y23" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="Z23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="AA23" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1755,26 +2390,38 @@
       <c r="I24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="Q24" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="R24" s="2">
+        <v>3743</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="V24" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M24" s="2">
+      <c r="W24" s="2">
         <v>3096</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="X24" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="Y24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="Z24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="AA24" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
@@ -1787,26 +2434,32 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="V25" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M25" s="2">
+      <c r="W25" s="2">
         <v>3097</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="X25" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="Y25" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="Z25" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="AA25" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
@@ -1825,26 +2478,38 @@
       <c r="I26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="Q26" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="R26" s="2">
+        <v>3753</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="V26" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="M26" s="2">
+      <c r="W26" s="2">
         <v>3098</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="X26" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="Y26" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="Z26" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="AA26" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
@@ -1863,26 +2528,38 @@
       <c r="I27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="Q27" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="R27" s="2">
+        <v>3754</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="V27" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M27" s="2">
+      <c r="W27" s="2">
         <v>3099</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="X27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="Y27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="Z27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q27" s="2" t="s">
+      <c r="AA27" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
@@ -1901,26 +2578,38 @@
       <c r="I28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="Q28" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="R28" s="2">
+        <v>3755</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="V28" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="M28" s="2">
+      <c r="W28" s="2">
         <v>3100</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="X28" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="Y28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="Z28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="AA28" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1939,26 +2628,38 @@
       <c r="I29" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="Q29" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="R29" s="2">
+        <v>3756</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="V29" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M29" s="2">
+      <c r="W29" s="2">
         <v>3101</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="Y29" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="Z29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="AA29" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -1980,11 +2681,23 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q30" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="R30" s="2">
+        <v>3757</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2003,26 +2716,38 @@
       <c r="I31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="Q31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="R31" s="2">
+        <v>3758</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="V31" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M31" s="2">
+      <c r="W31" s="2">
         <v>3102</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="X31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="Y31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="Z31" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="AA31" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2044,11 +2769,23 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="Q32" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="R32" s="2">
+        <v>3759</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2061,8 +2798,26 @@
       <c r="I33" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="Q33" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="R33" s="2">
+        <v>3760</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G34" s="2" t="s">
         <v>101</v>
       </c>
@@ -2072,8 +2827,26 @@
       <c r="I34" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="Q34" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="R34" s="2">
+        <v>3761</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G35" s="2" t="s">
         <v>106</v>
       </c>
@@ -2083,18 +2856,60 @@
       <c r="I35" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="Q35" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="R35" s="2">
+        <v>3762</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G38" s="2" t="s">
         <v>63</v>
       </c>
@@ -2104,8 +2919,38 @@
       <c r="I38" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="Q38" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="R38" s="2">
+        <v>3772</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="W38" s="2">
+        <v>3372</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y38" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z38" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA38" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G39" s="2" t="s">
         <v>66</v>
       </c>
@@ -2115,13 +2960,55 @@
       <c r="I39" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="Q39" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="R39" s="2">
+        <v>3773</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="W39" s="2">
+        <v>3373</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y39" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z39" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G41" s="2" t="s">
         <v>69</v>
       </c>
@@ -2131,8 +3018,38 @@
       <c r="I41" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="Q41" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="R41" s="2">
+        <v>3783</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="W41" s="2">
+        <v>3383</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="Y41" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z41" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA41" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G42" s="2" t="s">
         <v>73</v>
       </c>
@@ -2142,8 +3059,38 @@
       <c r="I42" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="Q42" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R42" s="2">
+        <v>3784</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="W42" s="2">
+        <v>3384</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G43" s="2" t="s">
         <v>76</v>
       </c>
@@ -2153,8 +3100,38 @@
       <c r="I43" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="Q43" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="R43" s="2">
+        <v>3785</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="W43" s="2">
+        <v>3385</v>
+      </c>
+      <c r="X43" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y43" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z43" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G44" s="2" t="s">
         <v>81</v>
       </c>
@@ -2164,8 +3141,38 @@
       <c r="I44" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="Q44" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="R44" s="2">
+        <v>3786</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="W44" s="2">
+        <v>3386</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G45" s="2" t="s">
         <v>84</v>
       </c>
@@ -2175,8 +3182,38 @@
       <c r="I45" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="Q45" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="R45" s="2">
+        <v>3787</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="W45" s="2">
+        <v>3387</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G46" s="2" t="s">
         <v>93</v>
       </c>
@@ -2186,8 +3223,38 @@
       <c r="I46" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="Q46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="R46" s="2">
+        <v>3788</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="W46" s="2">
+        <v>3388</v>
+      </c>
+      <c r="X46" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G47" s="2" t="s">
         <v>96</v>
       </c>
@@ -2197,8 +3264,38 @@
       <c r="I47" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="Q47" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="R47" s="2">
+        <v>3789</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="W47" s="2">
+        <v>3389</v>
+      </c>
+      <c r="X47" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G48" s="2" t="s">
         <v>99</v>
       </c>
@@ -2208,8 +3305,38 @@
       <c r="I48" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="Q48" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="R48" s="2">
+        <v>3790</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="V48" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="W48" s="2">
+        <v>3390</v>
+      </c>
+      <c r="X48" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="Y48" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z48" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="7:27" x14ac:dyDescent="0.3">
       <c r="G49" s="2" t="s">
         <v>102</v>
       </c>
@@ -2219,8 +3346,38 @@
       <c r="I49" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="Q49" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="R49" s="2">
+        <v>3791</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="W49" s="2">
+        <v>3391</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z49" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="7:27" x14ac:dyDescent="0.3">
       <c r="G50" s="2" t="s">
         <v>108</v>
       </c>
@@ -2230,17 +3387,61 @@
       <c r="I50" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="Q50" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="R50" s="2">
+        <v>3792</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="V50" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="W50" s="2">
+        <v>3392</v>
+      </c>
+      <c r="X50" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y50" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z50" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="7:27" x14ac:dyDescent="0.3">
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="L6:Q6"/>
+    <mergeCell ref="V6:AA6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="Q6:S6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2252,8 +3453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B135286-D673-4043-B681-3A5B7A012B1D}">
   <dimension ref="B6:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,9 +3814,13 @@
       <c r="G21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2633,9 +3838,13 @@
       <c r="G22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>

</xml_diff>

<commit_message>
Update PLC program and variable reference
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128A9ABB-D8EA-4C83-BFA1-32FD90D345FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1976B6E-CD25-458C-B1A2-535FEC44C794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="366">
   <si>
     <t>Effective Length</t>
   </si>
@@ -1118,6 +1118,12 @@
   </si>
   <si>
     <t>M320</t>
+  </si>
+  <si>
+    <t>Feeding Set Value Step 0 (Initial)</t>
+  </si>
+  <si>
+    <t>V3010</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:AA51"/>
+  <dimension ref="B6:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41:X50"/>
+    <sheetView tabSelected="1" topLeftCell="M5" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,13 +1732,13 @@
         <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>67</v>
+        <v>364</v>
       </c>
       <c r="H11" s="2">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>52</v>
+        <v>365</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>291</v>
@@ -1782,13 +1788,13 @@
         <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H12" s="2">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>292</v>
@@ -1826,13 +1832,13 @@
         <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H13" s="2">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>293</v>
@@ -1882,13 +1888,13 @@
         <v>31</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H14" s="2">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>294</v>
@@ -1938,13 +1944,13 @@
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H15" s="2">
-        <v>3527</v>
+        <v>3526</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>295</v>
@@ -1994,13 +2000,13 @@
         <v>164</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H16" s="2">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>296</v>
@@ -2044,13 +2050,13 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>297</v>
@@ -2100,13 +2106,13 @@
         <v>33</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H18" s="2">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>298</v>
@@ -2156,13 +2162,13 @@
         <v>34</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H19" s="2">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>299</v>
@@ -2200,13 +2206,13 @@
         <v>35</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H20" s="2">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>300</v>
@@ -2255,9 +2261,15 @@
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3532</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2331,15 +2343,9 @@
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="2">
-        <v>3542</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2382,13 +2388,13 @@
         <v>39</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H24" s="2">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -2431,9 +2437,15 @@
       <c r="D25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="2">
+        <v>3543</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2469,15 +2481,9 @@
       <c r="D26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="2">
-        <v>3553</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2520,13 +2526,13 @@
         <v>42</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H27" s="2">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -2570,13 +2576,13 @@
         <v>43</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H28" s="2">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2620,13 +2626,13 @@
         <v>44</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H29" s="2">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2670,13 +2676,13 @@
         <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H30" s="2">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2708,13 +2714,13 @@
         <v>46</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H31" s="2">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2758,13 +2764,13 @@
         <v>47</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H32" s="2">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2790,13 +2796,13 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H33" s="2">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -2819,13 +2825,13 @@
     </row>
     <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G34" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H34" s="2">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -2848,13 +2854,13 @@
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G35" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H35" s="2">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -2876,9 +2882,15 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3562</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2910,15 +2922,9 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="G38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" s="2">
-        <v>3572</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2952,13 +2958,13 @@
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H39" s="2">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
@@ -2992,9 +2998,15 @@
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="2">
+        <v>3573</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -3009,15 +3021,9 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="G41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41" s="2">
-        <v>3583</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3051,13 +3057,13 @@
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G42" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H42" s="2">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -3092,13 +3098,13 @@
     </row>
     <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G43" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H43" s="2">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -3133,13 +3139,13 @@
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G44" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H44" s="2">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -3174,13 +3180,13 @@
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G45" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H45" s="2">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
@@ -3215,13 +3221,13 @@
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G46" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H46" s="2">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
@@ -3256,13 +3262,13 @@
     </row>
     <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G47" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H47" s="2">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
@@ -3297,13 +3303,13 @@
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.3">
       <c r="G48" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H48" s="2">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
@@ -3338,13 +3344,13 @@
     </row>
     <row r="49" spans="7:27" x14ac:dyDescent="0.3">
       <c r="G49" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H49" s="2">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
@@ -3379,13 +3385,13 @@
     </row>
     <row r="50" spans="7:27" x14ac:dyDescent="0.3">
       <c r="G50" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H50" s="2">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
@@ -3419,9 +3425,15 @@
       </c>
     </row>
     <row r="51" spans="7:27" x14ac:dyDescent="0.3">
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="G51" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" s="2">
+        <v>3592</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3434,6 +3446,11 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
+    </row>
+    <row r="52" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
"Updated main.py, ref/CNC Pipe Bending Machine - Parameter Variables.xlsx, and screen_operate_manual.kv with various changes, including flag renames, added sensor flags, and UI layout adjustments."
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121A12C-E9D7-4B4A-B70A-CDF711DABAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C955762D-64CA-442C-B616-F793A0FB6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VAR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="423">
   <si>
     <t>Effective Length</t>
   </si>
@@ -1150,10 +1150,151 @@
     <t>Y22</t>
   </si>
   <si>
-    <t>Selenoid Valve Pneumatic Holder Up</t>
-  </si>
-  <si>
-    <t>Selenoid Valve Pneumatic Holder Down</t>
+    <t>Sensor Reed Clamp Close</t>
+  </si>
+  <si>
+    <t>X16</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>IO Servo</t>
+  </si>
+  <si>
+    <t>Single Selenoid</t>
+  </si>
+  <si>
+    <t>Double Selenoid</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Pneumatic Holder Top</t>
+  </si>
+  <si>
+    <t>Selenoid Valve Pneumatic Holder Bottom</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Y11</t>
+  </si>
+  <si>
+    <t>Y12</t>
+  </si>
+  <si>
+    <t>Y13</t>
+  </si>
+  <si>
+    <t>Y14</t>
+  </si>
+  <si>
+    <t>Y15</t>
+  </si>
+  <si>
+    <t>X17</t>
+  </si>
+  <si>
+    <t>X18</t>
+  </si>
+  <si>
+    <t>X19</t>
+  </si>
+  <si>
+    <t>X20</t>
+  </si>
+  <si>
+    <t>X21</t>
+  </si>
+  <si>
+    <t>X22</t>
+  </si>
+  <si>
+    <t>X23</t>
+  </si>
+  <si>
+    <t>X24</t>
+  </si>
+  <si>
+    <t>Y23</t>
+  </si>
+  <si>
+    <t>Y24</t>
+  </si>
+  <si>
+    <t>Sensor Reed Press Open</t>
+  </si>
+  <si>
+    <t>Sensor Proximity Origin Bend</t>
+  </si>
+  <si>
+    <t>Sensor Beam Reducer Bend</t>
+  </si>
+  <si>
+    <t>Sensor Reed Table Down (Min)</t>
+  </si>
+  <si>
+    <t>Sensor Reed Table Up (Max)</t>
+  </si>
+  <si>
+    <t>Sensor Reed Chuck Close</t>
+  </si>
+  <si>
+    <t>Sensor Proximity Reducer Feed</t>
+  </si>
+  <si>
+    <t>Sensor Proximity Origin Feed</t>
+  </si>
+  <si>
+    <t>M111</t>
+  </si>
+  <si>
+    <t>M112</t>
+  </si>
+  <si>
+    <t>M113</t>
+  </si>
+  <si>
+    <t>M114</t>
+  </si>
+  <si>
+    <t>M115</t>
+  </si>
+  <si>
+    <t>M116</t>
+  </si>
+  <si>
+    <t>M117</t>
+  </si>
+  <si>
+    <t>M118</t>
+  </si>
+  <si>
+    <t>M119</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>On</t>
   </si>
 </sst>
 </file>
@@ -1505,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:AA52"/>
+  <dimension ref="B6:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="Q10" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" topLeftCell="V6" workbookViewId="0">
+      <selection activeCell="AE21" sqref="AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,9 +1666,13 @@
     <col min="23" max="24" width="15.33203125" customWidth="1"/>
     <col min="25" max="26" width="10.21875" customWidth="1"/>
     <col min="27" max="27" width="10.5546875" customWidth="1"/>
+    <col min="30" max="30" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.33203125" customWidth="1"/>
+    <col min="33" max="34" width="10.21875" customWidth="1"/>
+    <col min="35" max="35" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>124</v>
       </c>
@@ -1556,8 +1701,16 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1612,8 +1765,26 @@
       <c r="AA7" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1662,8 +1833,26 @@
       <c r="AA8" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD8" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>3183</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1712,8 +1901,26 @@
       <c r="AA9" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD9" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>3184</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="10" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1750,8 +1957,26 @@
       <c r="AA10" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD10" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>3185</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1770,15 +1995,9 @@
       <c r="I11" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="M11" s="2">
-        <v>3623</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>241</v>
-      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
       <c r="Q11" s="2" t="s">
         <v>251</v>
       </c>
@@ -1806,8 +2025,26 @@
       <c r="AA11" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD11" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>3186</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1827,13 +2064,13 @@
         <v>52</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M12" s="2">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>252</v>
@@ -1850,8 +2087,26 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-    </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD12" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>3187</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1871,13 +2126,13 @@
         <v>53</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M13" s="2">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>253</v>
@@ -1906,8 +2161,26 @@
       <c r="AA13" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD13" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>3188</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1927,13 +2200,13 @@
         <v>54</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M14" s="2">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>254</v>
@@ -1962,8 +2235,26 @@
       <c r="AA14" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD14" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>3189</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1983,13 +2274,13 @@
         <v>55</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M15" s="2">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>255</v>
@@ -2018,8 +2309,26 @@
       <c r="AA15" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD15" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>3190</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>163</v>
       </c>
@@ -2039,13 +2348,13 @@
         <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M16" s="2">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>256</v>
@@ -2074,8 +2383,26 @@
       <c r="AA16" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD16" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>3191</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2089,13 +2416,13 @@
         <v>57</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M17" s="2">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>257</v>
@@ -2124,8 +2451,14 @@
       <c r="AA17" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+    </row>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2145,13 +2478,13 @@
         <v>58</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M18" s="2">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>258</v>
@@ -2180,8 +2513,14 @@
       <c r="AA18" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+    </row>
+    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2201,13 +2540,13 @@
         <v>59</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M19" s="2">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>259</v>
@@ -2232,8 +2571,14 @@
       <c r="AA19" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+    </row>
+    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
@@ -2253,13 +2598,13 @@
         <v>60</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M20" s="2">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>260</v>
@@ -2284,8 +2629,14 @@
       <c r="AA20" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+    </row>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
@@ -2304,9 +2655,15 @@
       <c r="I21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M21" s="2">
+        <v>3632</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -2316,8 +2673,14 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+    </row>
+    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
@@ -2342,8 +2705,14 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+    </row>
+    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
@@ -2386,8 +2755,14 @@
       <c r="AA23" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+    </row>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2436,8 +2811,14 @@
       <c r="AA24" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+    </row>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
@@ -2480,8 +2861,14 @@
       <c r="AA25" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+    </row>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
@@ -2524,8 +2911,14 @@
       <c r="AA26" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+    </row>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
@@ -2574,8 +2967,14 @@
       <c r="AA27" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+    </row>
+    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
@@ -2624,8 +3023,14 @@
       <c r="AA28" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+    </row>
+    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
@@ -2674,8 +3079,14 @@
       <c r="AA29" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+    </row>
+    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -2724,8 +3135,14 @@
       <c r="AA30" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+    </row>
+    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2774,8 +3191,14 @@
       <c r="AA31" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
+    </row>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2824,8 +3247,14 @@
       <c r="AA32" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+    </row>
+    <row r="33" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2856,8 +3285,14 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
-    </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+    </row>
+    <row r="34" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G34" s="2" t="s">
         <v>98</v>
       </c>
@@ -2897,8 +3332,14 @@
       <c r="AA34" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+    </row>
+    <row r="35" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G35" s="2" t="s">
         <v>101</v>
       </c>
@@ -2926,8 +3367,14 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
-    </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2"/>
+      <c r="AI35" s="2"/>
+    </row>
+    <row r="36" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G36" s="2" t="s">
         <v>106</v>
       </c>
@@ -2949,8 +3396,14 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
-    </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+    </row>
+    <row r="37" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2966,8 +3419,14 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
-    </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="2"/>
+    </row>
+    <row r="38" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -3001,8 +3460,14 @@
       <c r="AA38" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+    </row>
+    <row r="39" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G39" s="2" t="s">
         <v>63</v>
       </c>
@@ -3042,8 +3507,14 @@
       <c r="AA39" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
+    </row>
+    <row r="40" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G40" s="2" t="s">
         <v>66</v>
       </c>
@@ -3065,8 +3536,14 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
-    </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+    </row>
+    <row r="41" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -3100,8 +3577,14 @@
       <c r="AA41" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="2"/>
+      <c r="AI41" s="2"/>
+    </row>
+    <row r="42" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G42" s="2" t="s">
         <v>69</v>
       </c>
@@ -3141,8 +3624,14 @@
       <c r="AA42" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+    </row>
+    <row r="43" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G43" s="2" t="s">
         <v>73</v>
       </c>
@@ -3182,8 +3671,14 @@
       <c r="AA43" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AI43" s="2"/>
+    </row>
+    <row r="44" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G44" s="2" t="s">
         <v>76</v>
       </c>
@@ -3223,8 +3718,14 @@
       <c r="AA44" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
+      <c r="AI44" s="2"/>
+    </row>
+    <row r="45" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G45" s="2" t="s">
         <v>81</v>
       </c>
@@ -3264,8 +3765,14 @@
       <c r="AA45" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+      <c r="AG45" s="2"/>
+      <c r="AH45" s="2"/>
+      <c r="AI45" s="2"/>
+    </row>
+    <row r="46" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G46" s="2" t="s">
         <v>84</v>
       </c>
@@ -3305,8 +3812,14 @@
       <c r="AA46" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="2"/>
+    </row>
+    <row r="47" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G47" s="2" t="s">
         <v>93</v>
       </c>
@@ -3346,8 +3859,14 @@
       <c r="AA47" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2"/>
+    </row>
+    <row r="48" spans="2:35" x14ac:dyDescent="0.3">
       <c r="G48" s="2" t="s">
         <v>96</v>
       </c>
@@ -3387,8 +3906,14 @@
       <c r="AA48" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="49" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+      <c r="AG48" s="2"/>
+      <c r="AH48" s="2"/>
+      <c r="AI48" s="2"/>
+    </row>
+    <row r="49" spans="7:35" x14ac:dyDescent="0.3">
       <c r="G49" s="2" t="s">
         <v>99</v>
       </c>
@@ -3428,8 +3953,14 @@
       <c r="AA49" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="50" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+      <c r="AG49" s="2"/>
+      <c r="AH49" s="2"/>
+      <c r="AI49" s="2"/>
+    </row>
+    <row r="50" spans="7:35" x14ac:dyDescent="0.3">
       <c r="G50" s="2" t="s">
         <v>102</v>
       </c>
@@ -3469,8 +4000,14 @@
       <c r="AA50" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="51" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="2"/>
+    </row>
+    <row r="51" spans="7:35" x14ac:dyDescent="0.3">
       <c r="G51" s="2" t="s">
         <v>108</v>
       </c>
@@ -3492,14 +4029,21 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
-    </row>
-    <row r="52" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="2"/>
+      <c r="AF51" s="2"/>
+      <c r="AG51" s="2"/>
+      <c r="AH51" s="2"/>
+      <c r="AI51" s="2"/>
+    </row>
+    <row r="52" spans="7:35" x14ac:dyDescent="0.3">
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="AD6:AI6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:AA6"/>
@@ -3514,10 +4058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B135286-D673-4043-B681-3A5B7A012B1D}">
-  <dimension ref="B6:N30"/>
+  <dimension ref="B6:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3529,7 +4073,7 @@
     <col min="9" max="9" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="13" width="10.21875" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -3610,7 +4154,9 @@
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -3634,7 +4180,9 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -3658,7 +4206,9 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -3682,7 +4232,9 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -3706,7 +4258,9 @@
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -3730,12 +4284,16 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>383</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -3748,12 +4306,16 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -3766,7 +4328,9 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
@@ -3785,7 +4349,9 @@
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3798,12 +4364,16 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -3816,12 +4386,16 @@
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -3834,35 +4408,35 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>197</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>193</v>
+        <v>388</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>389</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -3871,30 +4445,30 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>390</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>223</v>
-      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>362</v>
+        <v>391</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3902,41 +4476,43 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>224</v>
-      </c>
+      <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>285</v>
-      </c>
+      <c r="G24" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -3949,98 +4525,238 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="I25" s="2" t="s">
-        <v>286</v>
-      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
-        <v>365</v>
-      </c>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>374</v>
+      </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>375</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="I26" s="2" t="s">
-        <v>367</v>
+        <v>223</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="I27" s="2" t="s">
-        <v>374</v>
+        <v>224</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+      <c r="N27" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>405</v>
+      </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>395</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="I28" s="2" t="s">
-        <v>375</v>
+        <v>285</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>404</v>
+      </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>396</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="K29" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>408</v>
+      </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>397</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>366</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
"Added flag sequences and step arrays, updated Modbus client reads, and modified screen layouts for operate auto and manual screens."
</commit_message>
<xml_diff>
--- a/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
+++ b/ref/CNC Pipe Bending Machine - Parameter Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nur Jamiludin\Documents\GitHub\cnc_pipe_bending_machine\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C955762D-64CA-442C-B616-F793A0FB6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4F7696-4A73-4D13-BA0D-5B62FB26BB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="467">
   <si>
     <t>Effective Length</t>
   </si>
@@ -1295,6 +1295,138 @@
   </si>
   <si>
     <t>On</t>
+  </si>
+  <si>
+    <t>M61</t>
+  </si>
+  <si>
+    <t>M62</t>
+  </si>
+  <si>
+    <t>M71</t>
+  </si>
+  <si>
+    <t>M72</t>
+  </si>
+  <si>
+    <t>M73</t>
+  </si>
+  <si>
+    <t>M74</t>
+  </si>
+  <si>
+    <t>M75</t>
+  </si>
+  <si>
+    <t>M76</t>
+  </si>
+  <si>
+    <t>M77</t>
+  </si>
+  <si>
+    <t>M78</t>
+  </si>
+  <si>
+    <t>M79</t>
+  </si>
+  <si>
+    <t>M200</t>
+  </si>
+  <si>
+    <t>Flag Sequence Init 1</t>
+  </si>
+  <si>
+    <t>Flag Sequence Init 2</t>
+  </si>
+  <si>
+    <t>Flag Sequence 1</t>
+  </si>
+  <si>
+    <t>Flag Sequence 2</t>
+  </si>
+  <si>
+    <t>Flag Sequence 3</t>
+  </si>
+  <si>
+    <t>Flag Sequence 4</t>
+  </si>
+  <si>
+    <t>Flag Sequence 5</t>
+  </si>
+  <si>
+    <t>Flag Sequence 6</t>
+  </si>
+  <si>
+    <t>Flag Sequence 7</t>
+  </si>
+  <si>
+    <t>Flag Sequence 8</t>
+  </si>
+  <si>
+    <t>Flag Sequence 9</t>
+  </si>
+  <si>
+    <t>Flag Step 1</t>
+  </si>
+  <si>
+    <t>Flag Step 2</t>
+  </si>
+  <si>
+    <t>M201</t>
+  </si>
+  <si>
+    <t>Flag Step 3</t>
+  </si>
+  <si>
+    <t>M202</t>
+  </si>
+  <si>
+    <t>Flag Step 4</t>
+  </si>
+  <si>
+    <t>M203</t>
+  </si>
+  <si>
+    <t>Flag Step 5</t>
+  </si>
+  <si>
+    <t>M204</t>
+  </si>
+  <si>
+    <t>Flag Step 6</t>
+  </si>
+  <si>
+    <t>M205</t>
+  </si>
+  <si>
+    <t>Flag Step 7</t>
+  </si>
+  <si>
+    <t>M206</t>
+  </si>
+  <si>
+    <t>Flag Step 8</t>
+  </si>
+  <si>
+    <t>M207</t>
+  </si>
+  <si>
+    <t>Flag Step 9</t>
+  </si>
+  <si>
+    <t>M208</t>
+  </si>
+  <si>
+    <t>Flag Step 10</t>
+  </si>
+  <si>
+    <t>M209</t>
+  </si>
+  <si>
+    <t>M210</t>
+  </si>
+  <si>
+    <t>Flag Step 0</t>
   </si>
 </sst>
 </file>
@@ -1648,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:AI52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V6" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView tabSelected="1" topLeftCell="V19" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2571,9 +2703,15 @@
       <c r="AA19" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
+      <c r="AD19" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>3133</v>
+      </c>
+      <c r="AF19" s="2" t="s">
+        <v>423</v>
+      </c>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
@@ -2629,9 +2767,15 @@
       <c r="AA20" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
+      <c r="AD20" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>3134</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>424</v>
+      </c>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
@@ -2673,9 +2817,15 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AF21" s="2"/>
+      <c r="AD21" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>3143</v>
+      </c>
+      <c r="AF21" s="2" t="s">
+        <v>425</v>
+      </c>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
@@ -2705,9 +2855,15 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
+      <c r="AD22" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="AE22" s="2">
+        <v>3144</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>426</v>
+      </c>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
@@ -2755,9 +2911,15 @@
       <c r="AA23" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
-      <c r="AF23" s="2"/>
+      <c r="AD23" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="AE23" s="2">
+        <v>3145</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
@@ -2811,9 +2973,15 @@
       <c r="AA24" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD24" s="2"/>
-      <c r="AE24" s="2"/>
-      <c r="AF24" s="2"/>
+      <c r="AD24" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE24" s="2">
+        <v>3146</v>
+      </c>
+      <c r="AF24" s="2" t="s">
+        <v>428</v>
+      </c>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
@@ -2861,9 +3029,15 @@
       <c r="AA25" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
-      <c r="AF25" s="2"/>
+      <c r="AD25" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="AE25" s="2">
+        <v>3147</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>429</v>
+      </c>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
@@ -2911,9 +3085,15 @@
       <c r="AA26" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD26" s="2"/>
-      <c r="AE26" s="2"/>
-      <c r="AF26" s="2"/>
+      <c r="AD26" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="AE26" s="2">
+        <v>3148</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>430</v>
+      </c>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
@@ -2967,9 +3147,15 @@
       <c r="AA27" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD27" s="2"/>
-      <c r="AE27" s="2"/>
-      <c r="AF27" s="2"/>
+      <c r="AD27" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="AE27" s="2">
+        <v>3149</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>431</v>
+      </c>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
@@ -3023,9 +3209,15 @@
       <c r="AA28" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD28" s="2"/>
-      <c r="AE28" s="2"/>
-      <c r="AF28" s="2"/>
+      <c r="AD28" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE28" s="2">
+        <v>3150</v>
+      </c>
+      <c r="AF28" s="2" t="s">
+        <v>432</v>
+      </c>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
@@ -3079,9 +3271,15 @@
       <c r="AA29" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD29" s="2"/>
-      <c r="AE29" s="2"/>
-      <c r="AF29" s="2"/>
+      <c r="AD29" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="AE29" s="2">
+        <v>3151</v>
+      </c>
+      <c r="AF29" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
@@ -3247,9 +3445,15 @@
       <c r="AA32" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD32" s="2"/>
-      <c r="AE32" s="2"/>
-      <c r="AF32" s="2"/>
+      <c r="AD32" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="AE32" s="2">
+        <v>3272</v>
+      </c>
+      <c r="AF32" s="2" t="s">
+        <v>434</v>
+      </c>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
@@ -3285,9 +3489,15 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
-      <c r="AD33" s="2"/>
-      <c r="AE33" s="2"/>
-      <c r="AF33" s="2"/>
+      <c r="AD33" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>3273</v>
+      </c>
+      <c r="AF33" s="2" t="s">
+        <v>448</v>
+      </c>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
@@ -3332,9 +3542,15 @@
       <c r="AA34" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2"/>
+      <c r="AD34" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="AE34" s="2">
+        <v>3274</v>
+      </c>
+      <c r="AF34" s="2" t="s">
+        <v>450</v>
+      </c>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
@@ -3367,9 +3583,15 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2"/>
+      <c r="AD35" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE35" s="2">
+        <v>3275</v>
+      </c>
+      <c r="AF35" s="2" t="s">
+        <v>452</v>
+      </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
@@ -3396,9 +3618,15 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
-      <c r="AD36" s="2"/>
-      <c r="AE36" s="2"/>
-      <c r="AF36" s="2"/>
+      <c r="AD36" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE36" s="2">
+        <v>3276</v>
+      </c>
+      <c r="AF36" s="2" t="s">
+        <v>454</v>
+      </c>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
@@ -3419,9 +3647,15 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
-      <c r="AD37" s="2"/>
-      <c r="AE37" s="2"/>
-      <c r="AF37" s="2"/>
+      <c r="AD37" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>3277</v>
+      </c>
+      <c r="AF37" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
@@ -3460,9 +3694,15 @@
       <c r="AA38" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="2"/>
+      <c r="AD38" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="AE38" s="2">
+        <v>3278</v>
+      </c>
+      <c r="AF38" s="2" t="s">
+        <v>458</v>
+      </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
@@ -3507,9 +3747,15 @@
       <c r="AA39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
+      <c r="AD39" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="AE39" s="2">
+        <v>3279</v>
+      </c>
+      <c r="AF39" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
@@ -3536,9 +3782,15 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
-      <c r="AD40" s="2"/>
-      <c r="AE40" s="2"/>
-      <c r="AF40" s="2"/>
+      <c r="AD40" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>3280</v>
+      </c>
+      <c r="AF40" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
@@ -3577,9 +3829,15 @@
       <c r="AA41" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
+      <c r="AD41" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="AE41" s="2">
+        <v>3281</v>
+      </c>
+      <c r="AF41" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
@@ -3624,9 +3882,15 @@
       <c r="AA42" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
-      <c r="AF42" s="2"/>
+      <c r="AD42" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="AE42" s="2">
+        <v>3282</v>
+      </c>
+      <c r="AF42" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2"/>
@@ -4060,7 +4324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B135286-D673-4043-B681-3A5B7A012B1D}">
   <dimension ref="B6:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26:B34"/>
     </sheetView>
   </sheetViews>

</xml_diff>